<commit_message>
update plotting script, new plots, and fixed bug
</commit_message>
<xml_diff>
--- a/02_in_data/All_LRR_PRR_ligand_data.xlsx
+++ b/02_in_data/All_LRR_PRR_ligand_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ffd16e31ab085cd5/Krasevia_Lab/Project/01_peptide_ML_prediction/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5075" documentId="8_{762EC3FE-3198-8040-A112-7E9B61E2665E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DE43F591-6163-0647-805D-D87356677E98}"/>
+  <xr:revisionPtr revIDLastSave="5090" documentId="8_{762EC3FE-3198-8040-A112-7E9B61E2665E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1AC3728F-2FE2-5240-8ABF-807A11EB7E8E}"/>
   <bookViews>
-    <workbookView xWindow="13040" yWindow="500" windowWidth="22080" windowHeight="19540" xr2:uid="{5C5BCD9C-73C9-CF41-954E-ACA1A5D65A44}"/>
+    <workbookView xWindow="13660" yWindow="500" windowWidth="19940" windowHeight="19540" xr2:uid="{5C5BCD9C-73C9-CF41-954E-ACA1A5D65A44}"/>
   </bookViews>
   <sheets>
     <sheet name="Model_Building" sheetId="1" r:id="rId1"/>
@@ -7215,7 +7215,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -7279,18 +7279,6 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -7611,8 +7599,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFCDCA10-C1DF-E744-9AE5-5ECCA937B4BD}">
   <dimension ref="A1:O1317"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1291" zoomScale="138" zoomScaleNormal="122" workbookViewId="0">
-      <selection activeCell="N1101" sqref="N1101"/>
+    <sheetView tabSelected="1" topLeftCell="A540" zoomScale="50" zoomScaleNormal="201" workbookViewId="0">
+      <selection activeCell="E708" sqref="E708"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -37002,7 +36990,7 @@
         <v>29</v>
       </c>
       <c r="E654" s="1">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F654" s="1" t="s">
         <v>108</v>
@@ -37046,7 +37034,7 @@
         <v>29</v>
       </c>
       <c r="E655" s="1">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F655" s="1" t="s">
         <v>108</v>
@@ -37090,7 +37078,7 @@
         <v>29</v>
       </c>
       <c r="E656" s="1">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F656" s="1" t="s">
         <v>108</v>
@@ -37662,7 +37650,7 @@
         <v>29</v>
       </c>
       <c r="E669" s="1">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F669" s="1" t="s">
         <v>108</v>
@@ -37706,7 +37694,7 @@
         <v>29</v>
       </c>
       <c r="E670" s="1">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F670" s="1" t="s">
         <v>108</v>
@@ -37750,7 +37738,7 @@
         <v>29</v>
       </c>
       <c r="E671" s="1">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F671" s="1" t="s">
         <v>108</v>
@@ -38586,7 +38574,7 @@
         <v>29</v>
       </c>
       <c r="E690" s="1">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F690" s="1" t="s">
         <v>108</v>
@@ -38630,7 +38618,7 @@
         <v>29</v>
       </c>
       <c r="E691" s="1">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F691" s="1" t="s">
         <v>108</v>
@@ -38674,7 +38662,7 @@
         <v>29</v>
       </c>
       <c r="E692" s="1">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F692" s="1" t="s">
         <v>108</v>
@@ -39158,7 +39146,7 @@
         <v>29</v>
       </c>
       <c r="E703" s="1">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F703" s="1" t="s">
         <v>108</v>
@@ -39202,7 +39190,7 @@
         <v>29</v>
       </c>
       <c r="E704" s="1">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F704" s="1" t="s">
         <v>108</v>
@@ -39246,7 +39234,7 @@
         <v>29</v>
       </c>
       <c r="E705" s="1">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F705" s="1" t="s">
         <v>108</v>
@@ -39290,7 +39278,7 @@
         <v>29</v>
       </c>
       <c r="E706" s="1">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F706" s="1" t="s">
         <v>108</v>
@@ -39334,7 +39322,7 @@
         <v>29</v>
       </c>
       <c r="E707" s="1">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F707" s="1" t="s">
         <v>108</v>
@@ -39378,7 +39366,7 @@
         <v>29</v>
       </c>
       <c r="E708" s="1">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F708" s="1" t="s">
         <v>108</v>
@@ -65559,238 +65547,238 @@
         <v>1945</v>
       </c>
     </row>
-    <row r="1282" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1282" s="25" t="s">
+    <row r="1282" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A1282" s="5" t="s">
         <v>1946</v>
       </c>
-      <c r="B1282" s="26" t="s">
+      <c r="B1282" s="1" t="s">
         <v>1413</v>
       </c>
-      <c r="C1282" s="26" t="s">
+      <c r="C1282" s="1" t="s">
         <v>1414</v>
       </c>
-      <c r="D1282" s="26" t="s">
-        <v>29</v>
-      </c>
-      <c r="E1282" s="26">
+      <c r="D1282" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1282" s="1">
         <v>28</v>
       </c>
-      <c r="F1282" s="26" t="s">
+      <c r="F1282" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="G1282" s="26" t="s">
+      <c r="G1282" s="1" t="s">
         <v>1416</v>
       </c>
-      <c r="H1282" s="27" t="s">
+      <c r="H1282" s="15" t="s">
         <v>1415</v>
       </c>
-      <c r="I1282" s="26" t="s">
+      <c r="I1282" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="J1282" s="26">
-        <v>20</v>
-      </c>
-      <c r="K1282" s="26" t="s">
+      <c r="J1282" s="1">
+        <v>20</v>
+      </c>
+      <c r="K1282" s="1" t="s">
         <v>1010</v>
       </c>
-      <c r="L1282" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="M1282" s="26" t="s">
+      <c r="L1282" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M1282" s="1" t="s">
         <v>979</v>
       </c>
-      <c r="N1282" s="26" t="s">
+      <c r="N1282" s="1" t="s">
         <v>1950</v>
       </c>
-      <c r="O1282" s="26" t="s">
+      <c r="O1282" s="1" t="s">
         <v>1949</v>
       </c>
     </row>
-    <row r="1283" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1283" s="25" t="s">
+    <row r="1283" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A1283" s="5" t="s">
         <v>1946</v>
       </c>
-      <c r="B1283" s="26" t="s">
+      <c r="B1283" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="C1283" s="26" t="s">
+      <c r="C1283" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="D1283" s="26" t="s">
-        <v>29</v>
-      </c>
-      <c r="E1283" s="26">
+      <c r="D1283" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1283" s="1">
         <v>28</v>
       </c>
-      <c r="F1283" s="26" t="s">
+      <c r="F1283" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="G1283" s="26" t="s">
+      <c r="G1283" s="1" t="s">
         <v>527</v>
       </c>
-      <c r="H1283" s="25" t="s">
+      <c r="H1283" s="5" t="s">
         <v>528</v>
       </c>
-      <c r="I1283" s="26" t="s">
+      <c r="I1283" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="J1283" s="26">
-        <v>20</v>
-      </c>
-      <c r="K1283" s="26" t="s">
+      <c r="J1283" s="1">
+        <v>20</v>
+      </c>
+      <c r="K1283" s="1" t="s">
         <v>1010</v>
       </c>
-      <c r="L1283" s="26" t="s">
+      <c r="L1283" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="M1283" s="26" t="s">
+      <c r="M1283" s="1" t="s">
         <v>979</v>
       </c>
-      <c r="N1283" s="26" t="s">
+      <c r="N1283" s="1" t="s">
         <v>1950</v>
       </c>
-      <c r="O1283" s="26" t="s">
+      <c r="O1283" s="1" t="s">
         <v>1949</v>
       </c>
     </row>
-    <row r="1284" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1284" s="25" t="s">
+    <row r="1284" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A1284" s="5" t="s">
         <v>1946</v>
       </c>
-      <c r="B1284" s="26" t="s">
+      <c r="B1284" s="1" t="s">
         <v>1413</v>
       </c>
-      <c r="C1284" s="26" t="s">
+      <c r="C1284" s="1" t="s">
         <v>1414</v>
       </c>
-      <c r="D1284" s="26" t="s">
-        <v>29</v>
-      </c>
-      <c r="E1284" s="26">
+      <c r="D1284" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1284" s="1">
         <v>28</v>
       </c>
-      <c r="F1284" s="26" t="s">
+      <c r="F1284" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="G1284" s="26" t="s">
+      <c r="G1284" s="1" t="s">
         <v>1416</v>
       </c>
-      <c r="H1284" s="27" t="s">
+      <c r="H1284" s="15" t="s">
         <v>1415</v>
       </c>
-      <c r="I1284" s="26" t="s">
+      <c r="I1284" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="J1284" s="26">
-        <v>20</v>
-      </c>
-      <c r="K1284" s="26" t="s">
+      <c r="J1284" s="1">
+        <v>20</v>
+      </c>
+      <c r="K1284" s="1" t="s">
         <v>1947</v>
       </c>
-      <c r="L1284" s="26" t="s">
+      <c r="L1284" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="M1284" s="26" t="s">
+      <c r="M1284" s="1" t="s">
         <v>979</v>
       </c>
-      <c r="N1284" s="26" t="s">
+      <c r="N1284" s="1" t="s">
         <v>1950</v>
       </c>
-      <c r="O1284" s="26" t="s">
+      <c r="O1284" s="1" t="s">
         <v>1948</v>
       </c>
     </row>
-    <row r="1285" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1285" s="25" t="s">
+    <row r="1285" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A1285" s="5" t="s">
         <v>1946</v>
       </c>
-      <c r="B1285" s="26" t="s">
+      <c r="B1285" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="C1285" s="26" t="s">
+      <c r="C1285" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="D1285" s="26" t="s">
-        <v>29</v>
-      </c>
-      <c r="E1285" s="26">
+      <c r="D1285" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1285" s="1">
         <v>28</v>
       </c>
-      <c r="F1285" s="26" t="s">
+      <c r="F1285" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="G1285" s="26" t="s">
+      <c r="G1285" s="1" t="s">
         <v>527</v>
       </c>
-      <c r="H1285" s="25" t="s">
+      <c r="H1285" s="5" t="s">
         <v>528</v>
       </c>
-      <c r="I1285" s="26" t="s">
+      <c r="I1285" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="J1285" s="26">
-        <v>20</v>
-      </c>
-      <c r="K1285" s="26" t="s">
+      <c r="J1285" s="1">
+        <v>20</v>
+      </c>
+      <c r="K1285" s="1" t="s">
         <v>1947</v>
       </c>
-      <c r="L1285" s="26" t="s">
+      <c r="L1285" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="M1285" s="26" t="s">
+      <c r="M1285" s="1" t="s">
         <v>979</v>
       </c>
-      <c r="N1285" s="26" t="s">
+      <c r="N1285" s="1" t="s">
         <v>1950</v>
       </c>
-      <c r="O1285" s="26" t="s">
+      <c r="O1285" s="1" t="s">
         <v>1948</v>
       </c>
     </row>
-    <row r="1286" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1286" s="25" t="s">
+    <row r="1286" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A1286" s="5" t="s">
         <v>1946</v>
       </c>
-      <c r="B1286" s="26" t="s">
+      <c r="B1286" s="1" t="s">
         <v>1413</v>
       </c>
-      <c r="C1286" s="26" t="s">
+      <c r="C1286" s="1" t="s">
         <v>1414</v>
       </c>
-      <c r="D1286" s="26" t="s">
-        <v>29</v>
-      </c>
-      <c r="E1286" s="26">
+      <c r="D1286" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1286" s="1">
         <v>28</v>
       </c>
-      <c r="F1286" s="26" t="s">
+      <c r="F1286" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="G1286" s="26" t="s">
+      <c r="G1286" s="1" t="s">
         <v>1416</v>
       </c>
-      <c r="H1286" s="27" t="s">
+      <c r="H1286" s="15" t="s">
         <v>1415</v>
       </c>
-      <c r="I1286" s="26" t="s">
+      <c r="I1286" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="J1286" s="26">
+      <c r="J1286" s="1">
         <v>8</v>
       </c>
-      <c r="K1286" s="26" t="s">
+      <c r="K1286" s="1" t="s">
         <v>1192</v>
       </c>
-      <c r="L1286" s="26" t="s">
+      <c r="L1286" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="M1286" s="26" t="s">
+      <c r="M1286" s="1" t="s">
         <v>979</v>
       </c>
-      <c r="N1286" s="26" t="s">
+      <c r="N1286" s="1" t="s">
         <v>1950</v>
       </c>
-      <c r="O1286" s="26" t="s">
+      <c r="O1286" s="1" t="s">
         <v>1193</v>
       </c>
     </row>
@@ -66785,7 +66773,7 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="27" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G27" s="29" t="s">
+      <c r="G27" s="25" t="s">
         <v>1954</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update Model_Validation Immunogenicity outcomes
</commit_message>
<xml_diff>
--- a/02_in_data/All_LRR_PRR_ligand_data.xlsx
+++ b/02_in_data/All_LRR_PRR_ligand_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ffd16e31ab085cd5/Krasevia_Lab/Project/01_peptide_ML_prediction/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniellestevens/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6024" documentId="8_{762EC3FE-3198-8040-A112-7E9B61E2665E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2F268835-855C-E14F-8D14-FD3DD978101C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9FE9B50-CBB0-2843-9B8F-77E6E29E137E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="41480" yWindow="25920" windowWidth="33600" windowHeight="14980" activeTab="2" xr2:uid="{5C5BCD9C-73C9-CF41-954E-ACA1A5D65A44}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19036" uniqueCount="2211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19060" uniqueCount="2211">
   <si>
     <t>Plant species</t>
   </si>
@@ -7757,7 +7757,7 @@
     <t>Cm csp22-3</t>
   </si>
   <si>
-    <t>TBD</t>
+    <t>NT</t>
   </si>
 </sst>
 </file>
@@ -7981,7 +7981,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -71623,8 +71623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCBE6D4C-D737-5E4F-BBF1-96687064E73B}">
   <dimension ref="A1:O131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="75" zoomScaleNormal="92" workbookViewId="0">
-      <selection activeCell="P60" sqref="P60"/>
+    <sheetView tabSelected="1" topLeftCell="B101" zoomScale="75" zoomScaleNormal="92" workbookViewId="0">
+      <selection activeCell="L138" sqref="L138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -71822,7 +71822,7 @@
         <v>150</v>
       </c>
       <c r="L4" s="9" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="M4" s="1" t="s">
         <v>116</v>
@@ -72010,7 +72010,7 @@
         <v>154</v>
       </c>
       <c r="L8" s="9" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="M8" s="1" t="s">
         <v>116</v>
@@ -72151,7 +72151,7 @@
         <v>157</v>
       </c>
       <c r="L11" s="9" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="M11" s="1" t="s">
         <v>116</v>
@@ -72479,7 +72479,7 @@
       <c r="K18" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="L18" s="26" t="s">
+      <c r="L18" s="9" t="s">
         <v>20</v>
       </c>
       <c r="M18" s="1" t="s">
@@ -72715,7 +72715,7 @@
         <v>169</v>
       </c>
       <c r="L23" s="9" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="M23" s="1" t="s">
         <v>116</v>
@@ -72949,8 +72949,8 @@
       <c r="K28" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="L28" s="25" t="s">
-        <v>2210</v>
+      <c r="L28" s="9" t="s">
+        <v>20</v>
       </c>
       <c r="M28" s="1" t="s">
         <v>116</v>
@@ -73466,7 +73466,7 @@
       <c r="K39" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="L39" s="26" t="s">
+      <c r="L39" s="9" t="s">
         <v>1557</v>
       </c>
       <c r="M39" s="1" t="s">
@@ -73560,8 +73560,8 @@
       <c r="K41" s="9" t="s">
         <v>188</v>
       </c>
-      <c r="L41" s="25" t="s">
-        <v>2210</v>
+      <c r="L41" s="9" t="s">
+        <v>1557</v>
       </c>
       <c r="M41" s="1" t="s">
         <v>116</v>
@@ -73654,7 +73654,7 @@
       <c r="K43" s="9" t="s">
         <v>190</v>
       </c>
-      <c r="L43" s="26" t="s">
+      <c r="L43" s="9" t="s">
         <v>38</v>
       </c>
       <c r="M43" s="1" t="s">
@@ -73749,7 +73749,7 @@
         <v>192</v>
       </c>
       <c r="L45" s="9" t="s">
-        <v>1557</v>
+        <v>38</v>
       </c>
       <c r="M45" s="1" t="s">
         <v>116</v>
@@ -73984,7 +73984,7 @@
         <v>197</v>
       </c>
       <c r="L50" s="9" t="s">
-        <v>1557</v>
+        <v>38</v>
       </c>
       <c r="M50" s="1" t="s">
         <v>116</v>
@@ -74124,7 +74124,7 @@
       <c r="K53" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="L53" s="26" t="s">
+      <c r="L53" s="9" t="s">
         <v>1557</v>
       </c>
       <c r="M53" s="1" t="s">
@@ -74218,8 +74218,8 @@
       <c r="K55" s="9" t="s">
         <v>202</v>
       </c>
-      <c r="L55" s="25" t="s">
-        <v>2210</v>
+      <c r="L55" s="9" t="s">
+        <v>1557</v>
       </c>
       <c r="M55" s="1" t="s">
         <v>116</v>
@@ -74359,8 +74359,8 @@
       <c r="K58" s="9" t="s">
         <v>205</v>
       </c>
-      <c r="L58" s="25" t="s">
-        <v>2210</v>
+      <c r="L58" s="9" t="s">
+        <v>1557</v>
       </c>
       <c r="M58" s="1" t="s">
         <v>116</v>
@@ -74688,8 +74688,8 @@
       <c r="K65" s="9" t="s">
         <v>243</v>
       </c>
-      <c r="L65" s="25" t="s">
-        <v>2210</v>
+      <c r="L65" s="9" t="s">
+        <v>38</v>
       </c>
       <c r="M65" s="1" t="s">
         <v>116</v>
@@ -74782,7 +74782,7 @@
       <c r="K67" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="L67" s="26" t="s">
+      <c r="L67" s="9" t="s">
         <v>20</v>
       </c>
       <c r="M67" s="1" t="s">
@@ -74829,8 +74829,8 @@
       <c r="K68" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="L68" s="26" t="s">
-        <v>20</v>
+      <c r="L68" s="9" t="s">
+        <v>38</v>
       </c>
       <c r="M68" s="1" t="s">
         <v>116</v>
@@ -74876,7 +74876,9 @@
       <c r="K69" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="L69" s="26"/>
+      <c r="L69" s="9" t="s">
+        <v>38</v>
+      </c>
       <c r="M69" s="1" t="s">
         <v>116</v>
       </c>
@@ -74921,7 +74923,9 @@
       <c r="K70" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="L70" s="26"/>
+      <c r="L70" s="9" t="s">
+        <v>38</v>
+      </c>
       <c r="M70" s="1" t="s">
         <v>116</v>
       </c>
@@ -74966,7 +74970,7 @@
       <c r="K71" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="L71" s="26" t="s">
+      <c r="L71" s="9" t="s">
         <v>38</v>
       </c>
       <c r="M71" s="1" t="s">
@@ -75013,7 +75017,7 @@
       <c r="K72" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="L72" s="26" t="s">
+      <c r="L72" s="9" t="s">
         <v>38</v>
       </c>
       <c r="M72" s="1" t="s">
@@ -75060,7 +75064,9 @@
       <c r="K73" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="L73" s="26"/>
+      <c r="L73" s="9" t="s">
+        <v>38</v>
+      </c>
       <c r="M73" s="1" t="s">
         <v>116</v>
       </c>
@@ -75105,7 +75111,9 @@
       <c r="K74" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="L74" s="26"/>
+      <c r="L74" s="25" t="s">
+        <v>2210</v>
+      </c>
       <c r="M74" s="1" t="s">
         <v>116</v>
       </c>
@@ -75150,7 +75158,7 @@
       <c r="K75" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="L75" s="26" t="s">
+      <c r="L75" s="9" t="s">
         <v>20</v>
       </c>
       <c r="M75" s="1" t="s">
@@ -75197,7 +75205,9 @@
       <c r="K76" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="L76" s="26"/>
+      <c r="L76" s="9" t="s">
+        <v>20</v>
+      </c>
       <c r="M76" s="1" t="s">
         <v>116</v>
       </c>
@@ -75242,7 +75252,7 @@
       <c r="K77" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="L77" s="26" t="s">
+      <c r="L77" s="9" t="s">
         <v>20</v>
       </c>
       <c r="M77" s="1" t="s">
@@ -75289,7 +75299,9 @@
       <c r="K78" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="L78" s="26"/>
+      <c r="L78" s="9" t="s">
+        <v>20</v>
+      </c>
       <c r="M78" s="1" t="s">
         <v>116</v>
       </c>
@@ -75334,7 +75346,7 @@
       <c r="K79" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="L79" s="26" t="s">
+      <c r="L79" s="9" t="s">
         <v>38</v>
       </c>
       <c r="M79" s="1" t="s">
@@ -75381,7 +75393,7 @@
       <c r="K80" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="L80" s="26" t="s">
+      <c r="L80" s="9" t="s">
         <v>20</v>
       </c>
       <c r="M80" s="1" t="s">
@@ -75428,7 +75440,7 @@
       <c r="K81" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="L81" s="26" t="s">
+      <c r="L81" s="9" t="s">
         <v>1557</v>
       </c>
       <c r="M81" s="1" t="s">
@@ -75475,7 +75487,9 @@
       <c r="K82" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="L82" s="26"/>
+      <c r="L82" s="25" t="s">
+        <v>2210</v>
+      </c>
       <c r="M82" s="1" t="s">
         <v>116</v>
       </c>
@@ -75520,7 +75534,7 @@
       <c r="K83" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="L83" s="26" t="s">
+      <c r="L83" s="9" t="s">
         <v>20</v>
       </c>
       <c r="M83" s="1" t="s">
@@ -75567,7 +75581,7 @@
       <c r="K84" s="9" t="s">
         <v>165</v>
       </c>
-      <c r="L84" s="26" t="s">
+      <c r="L84" s="9" t="s">
         <v>1557</v>
       </c>
       <c r="M84" s="1" t="s">
@@ -75614,7 +75628,9 @@
       <c r="K85" s="9" t="s">
         <v>166</v>
       </c>
-      <c r="L85" s="26"/>
+      <c r="L85" s="9" t="s">
+        <v>38</v>
+      </c>
       <c r="M85" s="1" t="s">
         <v>116</v>
       </c>
@@ -75659,7 +75675,7 @@
       <c r="K86" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="L86" s="26" t="s">
+      <c r="L86" s="9" t="s">
         <v>38</v>
       </c>
       <c r="M86" s="1" t="s">
@@ -75706,7 +75722,7 @@
       <c r="K87" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="L87" s="26" t="s">
+      <c r="L87" s="9" t="s">
         <v>38</v>
       </c>
       <c r="M87" s="1" t="s">
@@ -75753,7 +75769,9 @@
       <c r="K88" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="L88" s="26"/>
+      <c r="L88" s="9" t="s">
+        <v>38</v>
+      </c>
       <c r="M88" s="1" t="s">
         <v>116</v>
       </c>
@@ -75798,7 +75816,9 @@
       <c r="K89" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="L89" s="26"/>
+      <c r="L89" s="9" t="s">
+        <v>20</v>
+      </c>
       <c r="M89" s="1" t="s">
         <v>116</v>
       </c>
@@ -75843,7 +75863,9 @@
       <c r="K90" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="L90" s="26"/>
+      <c r="L90" s="9" t="s">
+        <v>20</v>
+      </c>
       <c r="M90" s="1" t="s">
         <v>116</v>
       </c>
@@ -75888,7 +75910,7 @@
       <c r="K91" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="L91" s="26" t="s">
+      <c r="L91" s="9" t="s">
         <v>38</v>
       </c>
       <c r="M91" s="1" t="s">
@@ -75935,7 +75957,9 @@
       <c r="K92" s="9" t="s">
         <v>173</v>
       </c>
-      <c r="L92" s="26"/>
+      <c r="L92" s="25" t="s">
+        <v>2210</v>
+      </c>
       <c r="M92" s="1" t="s">
         <v>116</v>
       </c>
@@ -75980,7 +76004,9 @@
       <c r="K93" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="L93" s="26"/>
+      <c r="L93" s="9" t="s">
+        <v>20</v>
+      </c>
       <c r="M93" s="1" t="s">
         <v>116</v>
       </c>
@@ -76025,7 +76051,7 @@
       <c r="K94" s="9" t="s">
         <v>176</v>
       </c>
-      <c r="L94" s="26" t="s">
+      <c r="L94" s="9" t="s">
         <v>20</v>
       </c>
       <c r="M94" s="1" t="s">
@@ -76072,7 +76098,9 @@
       <c r="K95" s="9" t="s">
         <v>177</v>
       </c>
-      <c r="L95" s="26"/>
+      <c r="L95" s="9" t="s">
+        <v>20</v>
+      </c>
       <c r="M95" s="1" t="s">
         <v>116</v>
       </c>
@@ -76117,7 +76145,7 @@
       <c r="K96" s="9" t="s">
         <v>178</v>
       </c>
-      <c r="L96" s="26" t="s">
+      <c r="L96" s="9" t="s">
         <v>38</v>
       </c>
       <c r="M96" s="1" t="s">
@@ -76164,7 +76192,7 @@
       <c r="K97" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="L97" s="26" t="s">
+      <c r="L97" s="9" t="s">
         <v>38</v>
       </c>
       <c r="M97" s="1" t="s">
@@ -76211,7 +76239,7 @@
       <c r="K98" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="L98" s="26" t="s">
+      <c r="L98" s="9" t="s">
         <v>20</v>
       </c>
       <c r="M98" s="1" t="s">
@@ -76258,7 +76286,7 @@
       <c r="K99" s="9" t="s">
         <v>182</v>
       </c>
-      <c r="L99" s="26" t="s">
+      <c r="L99" s="9" t="s">
         <v>38</v>
       </c>
       <c r="M99" s="1" t="s">
@@ -76305,7 +76333,7 @@
       <c r="K100" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="L100" s="26" t="s">
+      <c r="L100" s="9" t="s">
         <v>38</v>
       </c>
       <c r="M100" s="1" t="s">
@@ -76352,7 +76380,9 @@
       <c r="K101" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="L101" s="26"/>
+      <c r="L101" s="25" t="s">
+        <v>2210</v>
+      </c>
       <c r="M101" s="1" t="s">
         <v>116</v>
       </c>
@@ -76397,7 +76427,7 @@
       <c r="K102" s="9" t="s">
         <v>184</v>
       </c>
-      <c r="L102" s="26" t="s">
+      <c r="L102" s="9" t="s">
         <v>1557</v>
       </c>
       <c r="M102" s="1" t="s">
@@ -76444,7 +76474,7 @@
       <c r="K103" s="9" t="s">
         <v>185</v>
       </c>
-      <c r="L103" s="26" t="s">
+      <c r="L103" s="9" t="s">
         <v>1557</v>
       </c>
       <c r="M103" s="1" t="s">
@@ -76491,7 +76521,7 @@
       <c r="K104" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="L104" s="26" t="s">
+      <c r="L104" s="9" t="s">
         <v>1557</v>
       </c>
       <c r="M104" s="1" t="s">
@@ -76538,7 +76568,9 @@
       <c r="K105" s="9" t="s">
         <v>187</v>
       </c>
-      <c r="L105" s="26"/>
+      <c r="L105" s="9" t="s">
+        <v>1557</v>
+      </c>
       <c r="M105" s="1" t="s">
         <v>116</v>
       </c>
@@ -76583,7 +76615,9 @@
       <c r="K106" s="9" t="s">
         <v>188</v>
       </c>
-      <c r="L106" s="26"/>
+      <c r="L106" s="25" t="s">
+        <v>2210</v>
+      </c>
       <c r="M106" s="1" t="s">
         <v>116</v>
       </c>
@@ -76628,7 +76662,9 @@
       <c r="K107" s="9" t="s">
         <v>189</v>
       </c>
-      <c r="L107" s="26"/>
+      <c r="L107" s="25" t="s">
+        <v>2210</v>
+      </c>
       <c r="M107" s="1" t="s">
         <v>116</v>
       </c>
@@ -76673,7 +76709,7 @@
       <c r="K108" s="9" t="s">
         <v>190</v>
       </c>
-      <c r="L108" s="26" t="s">
+      <c r="L108" s="9" t="s">
         <v>20</v>
       </c>
       <c r="M108" s="1" t="s">
@@ -76720,7 +76756,7 @@
       <c r="K109" s="9" t="s">
         <v>191</v>
       </c>
-      <c r="L109" s="26" t="s">
+      <c r="L109" s="9" t="s">
         <v>1557</v>
       </c>
       <c r="M109" s="1" t="s">
@@ -76767,7 +76803,7 @@
       <c r="K110" s="9" t="s">
         <v>192</v>
       </c>
-      <c r="L110" s="26" t="s">
+      <c r="L110" s="9" t="s">
         <v>20</v>
       </c>
       <c r="M110" s="1" t="s">
@@ -76814,7 +76850,7 @@
       <c r="K111" s="9" t="s">
         <v>193</v>
       </c>
-      <c r="L111" s="26" t="s">
+      <c r="L111" s="9" t="s">
         <v>1557</v>
       </c>
       <c r="M111" s="1" t="s">
@@ -76861,7 +76897,7 @@
       <c r="K112" s="9" t="s">
         <v>194</v>
       </c>
-      <c r="L112" s="26" t="s">
+      <c r="L112" s="9" t="s">
         <v>38</v>
       </c>
       <c r="M112" s="1" t="s">
@@ -76908,8 +76944,8 @@
       <c r="K113" s="9" t="s">
         <v>195</v>
       </c>
-      <c r="L113" s="26" t="s">
-        <v>1557</v>
+      <c r="L113" s="9" t="s">
+        <v>38</v>
       </c>
       <c r="M113" s="1" t="s">
         <v>116</v>
@@ -76955,7 +76991,7 @@
       <c r="K114" s="9" t="s">
         <v>196</v>
       </c>
-      <c r="L114" s="26" t="s">
+      <c r="L114" s="9" t="s">
         <v>1557</v>
       </c>
       <c r="M114" s="1" t="s">
@@ -77002,7 +77038,7 @@
       <c r="K115" s="9" t="s">
         <v>197</v>
       </c>
-      <c r="L115" s="26" t="s">
+      <c r="L115" s="9" t="s">
         <v>1557</v>
       </c>
       <c r="M115" s="1" t="s">
@@ -77049,7 +77085,7 @@
       <c r="K116" s="9" t="s">
         <v>198</v>
       </c>
-      <c r="L116" s="26" t="s">
+      <c r="L116" s="9" t="s">
         <v>1557</v>
       </c>
       <c r="M116" s="1" t="s">
@@ -77096,7 +77132,7 @@
       <c r="K117" s="9" t="s">
         <v>199</v>
       </c>
-      <c r="L117" s="26" t="s">
+      <c r="L117" s="9" t="s">
         <v>1557</v>
       </c>
       <c r="M117" s="1" t="s">
@@ -77143,7 +77179,7 @@
       <c r="K118" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="L118" s="26" t="s">
+      <c r="L118" s="9" t="s">
         <v>1557</v>
       </c>
       <c r="M118" s="1" t="s">
@@ -77190,7 +77226,7 @@
       <c r="K119" s="9" t="s">
         <v>201</v>
       </c>
-      <c r="L119" s="26" t="s">
+      <c r="L119" s="9" t="s">
         <v>1557</v>
       </c>
       <c r="M119" s="1" t="s">
@@ -77237,7 +77273,7 @@
       <c r="K120" s="9" t="s">
         <v>202</v>
       </c>
-      <c r="L120" s="26" t="s">
+      <c r="L120" s="9" t="s">
         <v>1557</v>
       </c>
       <c r="M120" s="1" t="s">
@@ -77284,7 +77320,7 @@
       <c r="K121" s="9" t="s">
         <v>203</v>
       </c>
-      <c r="L121" s="26" t="s">
+      <c r="L121" s="9" t="s">
         <v>1557</v>
       </c>
       <c r="M121" s="1" t="s">
@@ -77331,7 +77367,7 @@
       <c r="K122" s="9" t="s">
         <v>204</v>
       </c>
-      <c r="L122" s="26" t="s">
+      <c r="L122" s="9" t="s">
         <v>1557</v>
       </c>
       <c r="M122" s="1" t="s">
@@ -77378,7 +77414,9 @@
       <c r="K123" s="9" t="s">
         <v>205</v>
       </c>
-      <c r="L123" s="26"/>
+      <c r="L123" s="9" t="s">
+        <v>38</v>
+      </c>
       <c r="M123" s="1" t="s">
         <v>116</v>
       </c>
@@ -77423,7 +77461,7 @@
       <c r="K124" s="9" t="s">
         <v>206</v>
       </c>
-      <c r="L124" s="26" t="s">
+      <c r="L124" s="9" t="s">
         <v>20</v>
       </c>
       <c r="M124" s="1" t="s">
@@ -77470,7 +77508,9 @@
       <c r="K125" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="L125" s="26"/>
+      <c r="L125" s="25" t="s">
+        <v>2210</v>
+      </c>
       <c r="M125" s="1" t="s">
         <v>116</v>
       </c>
@@ -77515,7 +77555,9 @@
       <c r="K126" s="9" t="s">
         <v>208</v>
       </c>
-      <c r="L126" s="26"/>
+      <c r="L126" s="25" t="s">
+        <v>2210</v>
+      </c>
       <c r="M126" s="1" t="s">
         <v>116</v>
       </c>
@@ -77560,7 +77602,7 @@
       <c r="K127" s="9" t="s">
         <v>209</v>
       </c>
-      <c r="L127" s="26" t="s">
+      <c r="L127" s="9" t="s">
         <v>1557</v>
       </c>
       <c r="M127" s="1" t="s">
@@ -77607,7 +77649,9 @@
       <c r="K128" s="9" t="s">
         <v>210</v>
       </c>
-      <c r="L128" s="26"/>
+      <c r="L128" s="25" t="s">
+        <v>2210</v>
+      </c>
       <c r="M128" s="1" t="s">
         <v>116</v>
       </c>
@@ -77652,7 +77696,7 @@
       <c r="K129" s="9" t="s">
         <v>242</v>
       </c>
-      <c r="L129" s="26" t="s">
+      <c r="L129" s="9" t="s">
         <v>20</v>
       </c>
       <c r="M129" s="1" t="s">
@@ -77699,7 +77743,9 @@
       <c r="K130" s="9" t="s">
         <v>243</v>
       </c>
-      <c r="L130" s="26"/>
+      <c r="L130" s="25" t="s">
+        <v>2210</v>
+      </c>
       <c r="M130" s="1" t="s">
         <v>116</v>
       </c>
@@ -77744,7 +77790,9 @@
       <c r="K131" s="9" t="s">
         <v>244</v>
       </c>
-      <c r="L131" s="26"/>
+      <c r="L131" s="9" t="s">
+        <v>1557</v>
+      </c>
       <c r="M131" s="1" t="s">
         <v>116</v>
       </c>

</xml_diff>